<commit_message>
Týdenní správa dokumentace v Gitu
- Analýzy přesunuty do Analýza_sprint1
- doplnění všech souborů z teams
- doplnění zápisů v týdenní tabulce z teams
</commit_message>
<xml_diff>
--- a/dokumentace/RSP_UNICORN_tydny_prehledy_22_JV1(1).xlsx
+++ b/dokumentace/RSP_UNICORN_tydny_prehledy_22_JV1(1).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20391"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\voracek\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\schonova\RSP\UNICORN\dokumentace\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="181" documentId="13_ncr:1_{84AC1668-F742-4B5F-89F7-69B00B0BCA89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{81503006-AD87-4732-A57E-8DD33351FFD8}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{402E2995-4338-48CB-A115-3ECF72074857}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="3" activeTab="4" xr2:uid="{BC61F073-B12C-482B-97C0-FC4A34FC5EED}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" firstSheet="1" activeTab="4" xr2:uid="{BC61F073-B12C-482B-97C0-FC4A34FC5EED}"/>
   </bookViews>
   <sheets>
     <sheet name="19.-25.9." sheetId="2" r:id="rId1"/>
@@ -33,17 +33,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -119,7 +108,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -214,7 +203,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motiv Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -516,13 +505,13 @@
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.85546875" customWidth="1"/>
     <col min="3" max="9" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -541,7 +530,7 @@
       <c r="H1" s="4"/>
       <c r="I1" s="4"/>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="5"/>
       <c r="B2" s="7"/>
       <c r="C2" s="1" t="s">
@@ -566,7 +555,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
@@ -595,7 +584,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>13</v>
       </c>
@@ -624,7 +613,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>15</v>
       </c>
@@ -653,7 +642,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>17</v>
       </c>
@@ -682,7 +671,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>18</v>
       </c>
@@ -711,7 +700,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>19</v>
       </c>
@@ -759,13 +748,13 @@
       <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.85546875" customWidth="1"/>
     <col min="3" max="9" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -784,7 +773,7 @@
       <c r="H1" s="4"/>
       <c r="I1" s="4"/>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="5"/>
       <c r="B2" s="7"/>
       <c r="C2" s="1" t="s">
@@ -809,7 +798,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="str">
         <f>'19.-25.9.'!A3</f>
         <v>Miroslav Vávrů</v>
@@ -826,7 +815,7 @@
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="str">
         <f>'19.-25.9.'!A4</f>
         <v xml:space="preserve">Tomáš Došek </v>
@@ -843,7 +832,7 @@
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="str">
         <f>'19.-25.9.'!A5</f>
         <v>Nikola Schönová</v>
@@ -860,7 +849,7 @@
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="str">
         <f>'19.-25.9.'!A6</f>
         <v>David Henzl</v>
@@ -877,7 +866,7 @@
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="str">
         <f>'19.-25.9.'!A7</f>
         <v>Vojtěch Kordina</v>
@@ -894,7 +883,7 @@
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="str">
         <f>'19.-25.9.'!A8</f>
         <v>Jan Matoušek</v>
@@ -930,13 +919,13 @@
       <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.85546875" customWidth="1"/>
     <col min="3" max="9" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -955,7 +944,7 @@
       <c r="H1" s="4"/>
       <c r="I1" s="4"/>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="5"/>
       <c r="B2" s="7"/>
       <c r="C2" s="1" t="s">
@@ -980,7 +969,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="str">
         <f>'19.-25.9.'!A3</f>
         <v>Miroslav Vávrů</v>
@@ -997,7 +986,7 @@
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="str">
         <f>'19.-25.9.'!A4</f>
         <v xml:space="preserve">Tomáš Došek </v>
@@ -1014,7 +1003,7 @@
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="str">
         <f>'19.-25.9.'!A5</f>
         <v>Nikola Schönová</v>
@@ -1031,7 +1020,7 @@
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="str">
         <f>'19.-25.9.'!A6</f>
         <v>David Henzl</v>
@@ -1048,7 +1037,7 @@
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="str">
         <f>'19.-25.9.'!A7</f>
         <v>Vojtěch Kordina</v>
@@ -1065,7 +1054,7 @@
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="str">
         <f>'19.-25.9.'!A8</f>
         <v>Jan Matoušek</v>
@@ -1101,13 +1090,13 @@
       <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.85546875" customWidth="1"/>
     <col min="3" max="9" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1126,7 +1115,7 @@
       <c r="H1" s="4"/>
       <c r="I1" s="4"/>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="5"/>
       <c r="B2" s="7"/>
       <c r="C2" s="1" t="s">
@@ -1151,7 +1140,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="str">
         <f>'19.-25.9.'!A3</f>
         <v>Miroslav Vávrů</v>
@@ -1168,7 +1157,7 @@
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="str">
         <f>'19.-25.9.'!A4</f>
         <v xml:space="preserve">Tomáš Došek </v>
@@ -1185,7 +1174,7 @@
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="str">
         <f>'19.-25.9.'!A5</f>
         <v>Nikola Schönová</v>
@@ -1202,7 +1191,7 @@
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="str">
         <f>'19.-25.9.'!A6</f>
         <v>David Henzl</v>
@@ -1219,7 +1208,7 @@
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="str">
         <f>'19.-25.9.'!A7</f>
         <v>Vojtěch Kordina</v>
@@ -1236,7 +1225,7 @@
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="str">
         <f>'19.-25.9.'!A8</f>
         <v>Jan Matoušek</v>
@@ -1272,13 +1261,13 @@
       <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.85546875" customWidth="1"/>
     <col min="3" max="9" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1297,7 +1286,7 @@
       <c r="H1" s="4"/>
       <c r="I1" s="4"/>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="5"/>
       <c r="B2" s="7"/>
       <c r="C2" s="1" t="s">
@@ -1322,7 +1311,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="str">
         <f>'19.-25.9.'!A3</f>
         <v>Miroslav Vávrů</v>
@@ -1339,7 +1328,7 @@
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="str">
         <f>'19.-25.9.'!A4</f>
         <v xml:space="preserve">Tomáš Došek </v>
@@ -1356,7 +1345,7 @@
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="str">
         <f>'19.-25.9.'!A5</f>
         <v>Nikola Schönová</v>
@@ -1373,7 +1362,7 @@
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="str">
         <f>'19.-25.9.'!A6</f>
         <v>David Henzl</v>
@@ -1390,7 +1379,7 @@
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="str">
         <f>'19.-25.9.'!A7</f>
         <v>Vojtěch Kordina</v>
@@ -1407,7 +1396,7 @@
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="str">
         <f>'19.-25.9.'!A8</f>
         <v>Jan Matoušek</v>
@@ -1443,13 +1432,13 @@
       <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.85546875" customWidth="1"/>
     <col min="3" max="9" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1468,7 +1457,7 @@
       <c r="H1" s="4"/>
       <c r="I1" s="4"/>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="5"/>
       <c r="B2" s="7"/>
       <c r="C2" s="1" t="s">
@@ -1493,7 +1482,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="str">
         <f>'19.-25.9.'!A3</f>
         <v>Miroslav Vávrů</v>
@@ -1510,7 +1499,7 @@
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="str">
         <f>'19.-25.9.'!A4</f>
         <v xml:space="preserve">Tomáš Došek </v>
@@ -1527,7 +1516,7 @@
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="str">
         <f>'19.-25.9.'!A5</f>
         <v>Nikola Schönová</v>
@@ -1544,7 +1533,7 @@
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="str">
         <f>'19.-25.9.'!A6</f>
         <v>David Henzl</v>
@@ -1561,7 +1550,7 @@
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="str">
         <f>'19.-25.9.'!A7</f>
         <v>Vojtěch Kordina</v>
@@ -1578,7 +1567,7 @@
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="str">
         <f>'19.-25.9.'!A8</f>
         <v>Jan Matoušek</v>
@@ -1614,13 +1603,13 @@
       <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.85546875" customWidth="1"/>
     <col min="3" max="9" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1639,7 +1628,7 @@
       <c r="H1" s="4"/>
       <c r="I1" s="4"/>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="5"/>
       <c r="B2" s="7"/>
       <c r="C2" s="1" t="s">
@@ -1664,7 +1653,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="str">
         <f>'19.-25.9.'!A3</f>
         <v>Miroslav Vávrů</v>
@@ -1702,7 +1691,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="str">
         <f>'19.-25.9.'!A4</f>
         <v xml:space="preserve">Tomáš Došek </v>
@@ -1713,11 +1702,11 @@
       </c>
       <c r="C4" s="3">
         <f>'19.-25.9.'!C4+'26.9.- 2.10.'!C4+'3.10. - 9.10'!C4+'10.10 - 16.10.'!C4+'17.10. - 23.10.'!C4+'24.10. - 30.10.'!C4+'31.10. - 6.11.'!C4+'7.11. - 13.11.'!C4+'14.11. - 20.11.'!C4+'21.11. - 27.11.'!C4+'28.11. - 4.12.'!C4+'5.12. - 11.12.'!C4+'12.12. - 18.12.'!C4+'19.12. - 25.12.'!C4</f>
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D4" s="3">
         <f>'19.-25.9.'!D4+'26.9.- 2.10.'!D4+'3.10. - 9.10'!D4+'10.10 - 16.10.'!D4+'17.10. - 23.10.'!D4+'24.10. - 30.10.'!D4+'31.10. - 6.11.'!D4+'7.11. - 13.11.'!D4+'14.11. - 20.11.'!D4+'21.11. - 27.11.'!D4+'28.11. - 4.12.'!D4+'5.12. - 11.12.'!D4+'12.12. - 18.12.'!D4+'19.12. - 25.12.'!D4</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E4" s="3">
         <f>'19.-25.9.'!E4+'26.9.- 2.10.'!E4+'3.10. - 9.10'!E4+'10.10 - 16.10.'!E4+'17.10. - 23.10.'!E4+'24.10. - 30.10.'!E4+'31.10. - 6.11.'!E4+'7.11. - 13.11.'!E4+'14.11. - 20.11.'!E4+'21.11. - 27.11.'!E4+'28.11. - 4.12.'!E4+'5.12. - 11.12.'!E4+'12.12. - 18.12.'!E4+'19.12. - 25.12.'!E4</f>
@@ -1729,7 +1718,7 @@
       </c>
       <c r="G4" s="3">
         <f>'19.-25.9.'!G4+'26.9.- 2.10.'!G4+'3.10. - 9.10'!G4+'10.10 - 16.10.'!G4+'17.10. - 23.10.'!G4+'24.10. - 30.10.'!G4+'31.10. - 6.11.'!G4+'7.11. - 13.11.'!G4+'14.11. - 20.11.'!G4+'21.11. - 27.11.'!G4+'28.11. - 4.12.'!G4+'5.12. - 11.12.'!G4+'12.12. - 18.12.'!G4+'19.12. - 25.12.'!G4</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H4" s="3">
         <f>'19.-25.9.'!H4+'26.9.- 2.10.'!H4+'3.10. - 9.10'!H4+'10.10 - 16.10.'!H4+'17.10. - 23.10.'!H4+'24.10. - 30.10.'!H4+'31.10. - 6.11.'!H4+'7.11. - 13.11.'!H4+'14.11. - 20.11.'!H4+'21.11. - 27.11.'!H4+'28.11. - 4.12.'!H4+'5.12. - 11.12.'!H4+'12.12. - 18.12.'!H4+'19.12. - 25.12.'!H4</f>
@@ -1740,7 +1729,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="str">
         <f>'19.-25.9.'!A5</f>
         <v>Nikola Schönová</v>
@@ -1755,7 +1744,7 @@
       </c>
       <c r="D5" s="3">
         <f>'19.-25.9.'!D5+'26.9.- 2.10.'!D5+'3.10. - 9.10'!D5+'10.10 - 16.10.'!D5+'17.10. - 23.10.'!D5+'24.10. - 30.10.'!D5+'31.10. - 6.11.'!D5+'7.11. - 13.11.'!D5+'14.11. - 20.11.'!D5+'21.11. - 27.11.'!D5+'28.11. - 4.12.'!D5+'5.12. - 11.12.'!D5+'12.12. - 18.12.'!D5+'19.12. - 25.12.'!D5</f>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E5" s="3">
         <f>'19.-25.9.'!E5+'26.9.- 2.10.'!E5+'3.10. - 9.10'!E5+'10.10 - 16.10.'!E5+'17.10. - 23.10.'!E5+'24.10. - 30.10.'!E5+'31.10. - 6.11.'!E5+'7.11. - 13.11.'!E5+'14.11. - 20.11.'!E5+'21.11. - 27.11.'!E5+'28.11. - 4.12.'!E5+'5.12. - 11.12.'!E5+'12.12. - 18.12.'!E5+'19.12. - 25.12.'!E5</f>
@@ -1767,18 +1756,18 @@
       </c>
       <c r="G5" s="3">
         <f>'19.-25.9.'!G5+'26.9.- 2.10.'!G5+'3.10. - 9.10'!G5+'10.10 - 16.10.'!G5+'17.10. - 23.10.'!G5+'24.10. - 30.10.'!G5+'31.10. - 6.11.'!G5+'7.11. - 13.11.'!G5+'14.11. - 20.11.'!G5+'21.11. - 27.11.'!G5+'28.11. - 4.12.'!G5+'5.12. - 11.12.'!G5+'12.12. - 18.12.'!G5+'19.12. - 25.12.'!G5</f>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="H5" s="3">
         <f>'19.-25.9.'!H5+'26.9.- 2.10.'!H5+'3.10. - 9.10'!H5+'10.10 - 16.10.'!H5+'17.10. - 23.10.'!H5+'24.10. - 30.10.'!H5+'31.10. - 6.11.'!H5+'7.11. - 13.11.'!H5+'14.11. - 20.11.'!H5+'21.11. - 27.11.'!H5+'28.11. - 4.12.'!H5+'5.12. - 11.12.'!H5+'12.12. - 18.12.'!H5+'19.12. - 25.12.'!H5</f>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="I5" s="3">
         <f>'19.-25.9.'!I5+'26.9.- 2.10.'!I5+'3.10. - 9.10'!I5+'10.10 - 16.10.'!I5+'17.10. - 23.10.'!I5+'24.10. - 30.10.'!I5+'31.10. - 6.11.'!I5+'7.11. - 13.11.'!I5+'14.11. - 20.11.'!I5+'21.11. - 27.11.'!I5+'28.11. - 4.12.'!I5+'5.12. - 11.12.'!I5+'12.12. - 18.12.'!I5+'19.12. - 25.12.'!I5</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="str">
         <f>'19.-25.9.'!A6</f>
         <v>David Henzl</v>
@@ -1789,11 +1778,11 @@
       </c>
       <c r="C6" s="3">
         <f>'19.-25.9.'!C6+'26.9.- 2.10.'!C6+'3.10. - 9.10'!C6+'10.10 - 16.10.'!C6+'17.10. - 23.10.'!C6+'24.10. - 30.10.'!C6+'31.10. - 6.11.'!C6+'7.11. - 13.11.'!C6+'14.11. - 20.11.'!C6+'21.11. - 27.11.'!C6+'28.11. - 4.12.'!C6+'5.12. - 11.12.'!C6+'12.12. - 18.12.'!C6+'19.12. - 25.12.'!C6</f>
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D6" s="3">
         <f>'19.-25.9.'!D6+'26.9.- 2.10.'!D6+'3.10. - 9.10'!D6+'10.10 - 16.10.'!D6+'17.10. - 23.10.'!D6+'24.10. - 30.10.'!D6+'31.10. - 6.11.'!D6+'7.11. - 13.11.'!D6+'14.11. - 20.11.'!D6+'21.11. - 27.11.'!D6+'28.11. - 4.12.'!D6+'5.12. - 11.12.'!D6+'12.12. - 18.12.'!D6+'19.12. - 25.12.'!D6</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E6" s="3">
         <f>'19.-25.9.'!E6+'26.9.- 2.10.'!E6+'3.10. - 9.10'!E6+'10.10 - 16.10.'!E6+'17.10. - 23.10.'!E6+'24.10. - 30.10.'!E6+'31.10. - 6.11.'!E6+'7.11. - 13.11.'!E6+'14.11. - 20.11.'!E6+'21.11. - 27.11.'!E6+'28.11. - 4.12.'!E6+'5.12. - 11.12.'!E6+'12.12. - 18.12.'!E6+'19.12. - 25.12.'!E6</f>
@@ -1801,11 +1790,11 @@
       </c>
       <c r="F6" s="3">
         <f>'19.-25.9.'!F6+'26.9.- 2.10.'!F6+'3.10. - 9.10'!F6+'10.10 - 16.10.'!F6+'17.10. - 23.10.'!F6+'24.10. - 30.10.'!F6+'31.10. - 6.11.'!F6+'7.11. - 13.11.'!F6+'14.11. - 20.11.'!F6+'21.11. - 27.11.'!F6+'28.11. - 4.12.'!F6+'5.12. - 11.12.'!F6+'12.12. - 18.12.'!F6+'19.12. - 25.12.'!F6</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G6" s="3">
         <f>'19.-25.9.'!G6+'26.9.- 2.10.'!G6+'3.10. - 9.10'!G6+'10.10 - 16.10.'!G6+'17.10. - 23.10.'!G6+'24.10. - 30.10.'!G6+'31.10. - 6.11.'!G6+'7.11. - 13.11.'!G6+'14.11. - 20.11.'!G6+'21.11. - 27.11.'!G6+'28.11. - 4.12.'!G6+'5.12. - 11.12.'!G6+'12.12. - 18.12.'!G6+'19.12. - 25.12.'!G6</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H6" s="3">
         <f>'19.-25.9.'!H6+'26.9.- 2.10.'!H6+'3.10. - 9.10'!H6+'10.10 - 16.10.'!H6+'17.10. - 23.10.'!H6+'24.10. - 30.10.'!H6+'31.10. - 6.11.'!H6+'7.11. - 13.11.'!H6+'14.11. - 20.11.'!H6+'21.11. - 27.11.'!H6+'28.11. - 4.12.'!H6+'5.12. - 11.12.'!H6+'12.12. - 18.12.'!H6+'19.12. - 25.12.'!H6</f>
@@ -1813,10 +1802,10 @@
       </c>
       <c r="I6" s="3">
         <f>'19.-25.9.'!I6+'26.9.- 2.10.'!I6+'3.10. - 9.10'!I6+'10.10 - 16.10.'!I6+'17.10. - 23.10.'!I6+'24.10. - 30.10.'!I6+'31.10. - 6.11.'!I6+'7.11. - 13.11.'!I6+'14.11. - 20.11.'!I6+'21.11. - 27.11.'!I6+'28.11. - 4.12.'!I6+'5.12. - 11.12.'!I6+'12.12. - 18.12.'!I6+'19.12. - 25.12.'!I6</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="str">
         <f>'19.-25.9.'!A7</f>
         <v>Vojtěch Kordina</v>
@@ -1827,11 +1816,11 @@
       </c>
       <c r="C7" s="3">
         <f>'19.-25.9.'!C7+'26.9.- 2.10.'!C7+'3.10. - 9.10'!C7+'10.10 - 16.10.'!C7+'17.10. - 23.10.'!C7+'24.10. - 30.10.'!C7+'31.10. - 6.11.'!C7+'7.11. - 13.11.'!C7+'14.11. - 20.11.'!C7+'21.11. - 27.11.'!C7+'28.11. - 4.12.'!C7+'5.12. - 11.12.'!C7+'12.12. - 18.12.'!C7+'19.12. - 25.12.'!C7</f>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D7" s="3">
         <f>'19.-25.9.'!D7+'26.9.- 2.10.'!D7+'3.10. - 9.10'!D7+'10.10 - 16.10.'!D7+'17.10. - 23.10.'!D7+'24.10. - 30.10.'!D7+'31.10. - 6.11.'!D7+'7.11. - 13.11.'!D7+'14.11. - 20.11.'!D7+'21.11. - 27.11.'!D7+'28.11. - 4.12.'!D7+'5.12. - 11.12.'!D7+'12.12. - 18.12.'!D7+'19.12. - 25.12.'!D7</f>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E7" s="3">
         <f>'19.-25.9.'!E7+'26.9.- 2.10.'!E7+'3.10. - 9.10'!E7+'10.10 - 16.10.'!E7+'17.10. - 23.10.'!E7+'24.10. - 30.10.'!E7+'31.10. - 6.11.'!E7+'7.11. - 13.11.'!E7+'14.11. - 20.11.'!E7+'21.11. - 27.11.'!E7+'28.11. - 4.12.'!E7+'5.12. - 11.12.'!E7+'12.12. - 18.12.'!E7+'19.12. - 25.12.'!E7</f>
@@ -1839,22 +1828,22 @@
       </c>
       <c r="F7" s="3">
         <f>'19.-25.9.'!F7+'26.9.- 2.10.'!F7+'3.10. - 9.10'!F7+'10.10 - 16.10.'!F7+'17.10. - 23.10.'!F7+'24.10. - 30.10.'!F7+'31.10. - 6.11.'!F7+'7.11. - 13.11.'!F7+'14.11. - 20.11.'!F7+'21.11. - 27.11.'!F7+'28.11. - 4.12.'!F7+'5.12. - 11.12.'!F7+'12.12. - 18.12.'!F7+'19.12. - 25.12.'!F7</f>
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="G7" s="3">
         <f>'19.-25.9.'!G7+'26.9.- 2.10.'!G7+'3.10. - 9.10'!G7+'10.10 - 16.10.'!G7+'17.10. - 23.10.'!G7+'24.10. - 30.10.'!G7+'31.10. - 6.11.'!G7+'7.11. - 13.11.'!G7+'14.11. - 20.11.'!G7+'21.11. - 27.11.'!G7+'28.11. - 4.12.'!G7+'5.12. - 11.12.'!G7+'12.12. - 18.12.'!G7+'19.12. - 25.12.'!G7</f>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="H7" s="3">
         <f>'19.-25.9.'!H7+'26.9.- 2.10.'!H7+'3.10. - 9.10'!H7+'10.10 - 16.10.'!H7+'17.10. - 23.10.'!H7+'24.10. - 30.10.'!H7+'31.10. - 6.11.'!H7+'7.11. - 13.11.'!H7+'14.11. - 20.11.'!H7+'21.11. - 27.11.'!H7+'28.11. - 4.12.'!H7+'5.12. - 11.12.'!H7+'12.12. - 18.12.'!H7+'19.12. - 25.12.'!H7</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I7" s="3">
         <f>'19.-25.9.'!I7+'26.9.- 2.10.'!I7+'3.10. - 9.10'!I7+'10.10 - 16.10.'!I7+'17.10. - 23.10.'!I7+'24.10. - 30.10.'!I7+'31.10. - 6.11.'!I7+'7.11. - 13.11.'!I7+'14.11. - 20.11.'!I7+'21.11. - 27.11.'!I7+'28.11. - 4.12.'!I7+'5.12. - 11.12.'!I7+'12.12. - 18.12.'!I7+'19.12. - 25.12.'!I7</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="str">
         <f>'19.-25.9.'!A8</f>
         <v>Jan Matoušek</v>
@@ -1865,11 +1854,11 @@
       </c>
       <c r="C8" s="3">
         <f>'19.-25.9.'!C8+'26.9.- 2.10.'!C8+'3.10. - 9.10'!C8+'10.10 - 16.10.'!C8+'17.10. - 23.10.'!C8+'24.10. - 30.10.'!C8+'31.10. - 6.11.'!C8+'7.11. - 13.11.'!C8+'14.11. - 20.11.'!C8+'21.11. - 27.11.'!C8+'28.11. - 4.12.'!C8+'5.12. - 11.12.'!C8+'12.12. - 18.12.'!C8+'19.12. - 25.12.'!C8</f>
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D8" s="3">
         <f>'19.-25.9.'!D8+'26.9.- 2.10.'!D8+'3.10. - 9.10'!D8+'10.10 - 16.10.'!D8+'17.10. - 23.10.'!D8+'24.10. - 30.10.'!D8+'31.10. - 6.11.'!D8+'7.11. - 13.11.'!D8+'14.11. - 20.11.'!D8+'21.11. - 27.11.'!D8+'28.11. - 4.12.'!D8+'5.12. - 11.12.'!D8+'12.12. - 18.12.'!D8+'19.12. - 25.12.'!D8</f>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E8" s="3">
         <f>'19.-25.9.'!E8+'26.9.- 2.10.'!E8+'3.10. - 9.10'!E8+'10.10 - 16.10.'!E8+'17.10. - 23.10.'!E8+'24.10. - 30.10.'!E8+'31.10. - 6.11.'!E8+'7.11. - 13.11.'!E8+'14.11. - 20.11.'!E8+'21.11. - 27.11.'!E8+'28.11. - 4.12.'!E8+'5.12. - 11.12.'!E8+'12.12. - 18.12.'!E8+'19.12. - 25.12.'!E8</f>
@@ -1877,33 +1866,33 @@
       </c>
       <c r="F8" s="3">
         <f>'19.-25.9.'!F8+'26.9.- 2.10.'!F8+'3.10. - 9.10'!F8+'10.10 - 16.10.'!F8+'17.10. - 23.10.'!F8+'24.10. - 30.10.'!F8+'31.10. - 6.11.'!F8+'7.11. - 13.11.'!F8+'14.11. - 20.11.'!F8+'21.11. - 27.11.'!F8+'28.11. - 4.12.'!F8+'5.12. - 11.12.'!F8+'12.12. - 18.12.'!F8+'19.12. - 25.12.'!F8</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G8" s="3">
         <f>'19.-25.9.'!G8+'26.9.- 2.10.'!G8+'3.10. - 9.10'!G8+'10.10 - 16.10.'!G8+'17.10. - 23.10.'!G8+'24.10. - 30.10.'!G8+'31.10. - 6.11.'!G8+'7.11. - 13.11.'!G8+'14.11. - 20.11.'!G8+'21.11. - 27.11.'!G8+'28.11. - 4.12.'!G8+'5.12. - 11.12.'!G8+'12.12. - 18.12.'!G8+'19.12. - 25.12.'!G8</f>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="H8" s="3">
         <f>'19.-25.9.'!H8+'26.9.- 2.10.'!H8+'3.10. - 9.10'!H8+'10.10 - 16.10.'!H8+'17.10. - 23.10.'!H8+'24.10. - 30.10.'!H8+'31.10. - 6.11.'!H8+'7.11. - 13.11.'!H8+'14.11. - 20.11.'!H8+'21.11. - 27.11.'!H8+'28.11. - 4.12.'!H8+'5.12. - 11.12.'!H8+'12.12. - 18.12.'!H8+'19.12. - 25.12.'!H8</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I8" s="3">
         <f>'19.-25.9.'!I8+'26.9.- 2.10.'!I8+'3.10. - 9.10'!I8+'10.10 - 16.10.'!I8+'17.10. - 23.10.'!I8+'24.10. - 30.10.'!I8+'31.10. - 6.11.'!I8+'7.11. - 13.11.'!I8+'14.11. - 20.11.'!I8+'21.11. - 27.11.'!I8+'28.11. - 4.12.'!I8+'5.12. - 11.12.'!I8+'12.12. - 18.12.'!I8+'19.12. - 25.12.'!I8</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
         <v>20</v>
       </c>
       <c r="B9" s="9"/>
       <c r="C9" s="1">
         <f>SUM(C3:C8)</f>
-        <v>72</v>
+        <v>83</v>
       </c>
       <c r="D9" s="1">
         <f t="shared" ref="D9:I9" si="0">SUM(D3:D8)</f>
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="E9" s="1">
         <f t="shared" si="0"/>
@@ -1911,19 +1900,19 @@
       </c>
       <c r="F9" s="1">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="G9" s="1">
         <f t="shared" si="0"/>
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="H9" s="1">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="I9" s="1">
         <f t="shared" si="0"/>
-        <v>28</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -1946,13 +1935,13 @@
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.85546875" customWidth="1"/>
     <col min="3" max="9" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1971,7 +1960,7 @@
       <c r="H1" s="4"/>
       <c r="I1" s="4"/>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="5"/>
       <c r="B2" s="7"/>
       <c r="C2" s="1" t="s">
@@ -1996,7 +1985,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="str">
         <f>'19.-25.9.'!A3</f>
         <v>Miroslav Vávrů</v>
@@ -2027,7 +2016,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="str">
         <f>'19.-25.9.'!A4</f>
         <v xml:space="preserve">Tomáš Došek </v>
@@ -2058,7 +2047,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="str">
         <f>'19.-25.9.'!A5</f>
         <v>Nikola Schönová</v>
@@ -2089,7 +2078,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="str">
         <f>'19.-25.9.'!A6</f>
         <v>David Henzl</v>
@@ -2120,7 +2109,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="str">
         <f>'19.-25.9.'!A7</f>
         <v>Vojtěch Kordina</v>
@@ -2151,7 +2140,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="str">
         <f>'19.-25.9.'!A8</f>
         <v>Jan Matoušek</v>
@@ -2197,17 +2186,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A16EECFF-E792-46B6-96D2-EB978C7B193A}">
   <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.85546875" customWidth="1"/>
     <col min="3" max="9" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -2226,7 +2215,7 @@
       <c r="H1" s="4"/>
       <c r="I1" s="4"/>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="5"/>
       <c r="B2" s="7"/>
       <c r="C2" s="1" t="s">
@@ -2251,7 +2240,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="str">
         <f>'19.-25.9.'!A3</f>
         <v>Miroslav Vávrů</v>
@@ -2282,7 +2271,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="str">
         <f>'19.-25.9.'!A4</f>
         <v xml:space="preserve">Tomáš Došek </v>
@@ -2313,7 +2302,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="str">
         <f>'19.-25.9.'!A5</f>
         <v>Nikola Schönová</v>
@@ -2344,7 +2333,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="str">
         <f>'19.-25.9.'!A6</f>
         <v>David Henzl</v>
@@ -2375,7 +2364,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="str">
         <f>'19.-25.9.'!A7</f>
         <v>Vojtěch Kordina</v>
@@ -2406,7 +2395,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="str">
         <f>'19.-25.9.'!A8</f>
         <v>Jan Matoušek</v>
@@ -2452,17 +2441,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3C6F594-ED93-4F3B-9046-76E39F933269}">
   <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.85546875" customWidth="1"/>
     <col min="3" max="9" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -2481,7 +2470,7 @@
       <c r="H1" s="4"/>
       <c r="I1" s="4"/>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="5"/>
       <c r="B2" s="7"/>
       <c r="C2" s="1" t="s">
@@ -2506,7 +2495,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="str">
         <f>'19.-25.9.'!A3</f>
         <v>Miroslav Vávrů</v>
@@ -2537,7 +2526,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="str">
         <f>'19.-25.9.'!A4</f>
         <v xml:space="preserve">Tomáš Došek </v>
@@ -2554,7 +2543,7 @@
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="str">
         <f>'19.-25.9.'!A5</f>
         <v>Nikola Schönová</v>
@@ -2585,7 +2574,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="str">
         <f>'19.-25.9.'!A6</f>
         <v>David Henzl</v>
@@ -2594,15 +2583,29 @@
         <f>'19.-25.9.'!B6</f>
         <v>TM</v>
       </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-    </row>
-    <row r="7" spans="1:9">
+      <c r="C6" s="3">
+        <v>2</v>
+      </c>
+      <c r="D6" s="3">
+        <v>1</v>
+      </c>
+      <c r="E6" s="3">
+        <v>0</v>
+      </c>
+      <c r="F6" s="3">
+        <v>1</v>
+      </c>
+      <c r="G6" s="3">
+        <v>2</v>
+      </c>
+      <c r="H6" s="3">
+        <v>0</v>
+      </c>
+      <c r="I6" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="str">
         <f>'19.-25.9.'!A7</f>
         <v>Vojtěch Kordina</v>
@@ -2633,7 +2636,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="str">
         <f>'19.-25.9.'!A8</f>
         <v>Jan Matoušek</v>
@@ -2648,14 +2651,18 @@
       <c r="D8" s="3">
         <v>1</v>
       </c>
-      <c r="E8" s="3"/>
+      <c r="E8" s="3">
+        <v>0</v>
+      </c>
       <c r="F8" s="3">
         <v>1</v>
       </c>
       <c r="G8" s="3">
         <v>3</v>
       </c>
-      <c r="H8" s="3"/>
+      <c r="H8" s="3">
+        <v>0</v>
+      </c>
       <c r="I8" s="3">
         <v>2</v>
       </c>
@@ -2675,17 +2682,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD635C2F-4081-4474-9E0B-58BEE272740E}">
   <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5:I5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.85546875" customWidth="1"/>
     <col min="3" max="9" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -2704,7 +2711,7 @@
       <c r="H1" s="4"/>
       <c r="I1" s="4"/>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="5"/>
       <c r="B2" s="7"/>
       <c r="C2" s="1" t="s">
@@ -2729,7 +2736,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="str">
         <f>'19.-25.9.'!A3</f>
         <v>Miroslav Vávrů</v>
@@ -2746,7 +2753,7 @@
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="str">
         <f>'19.-25.9.'!A4</f>
         <v xml:space="preserve">Tomáš Došek </v>
@@ -2755,15 +2762,21 @@
         <f>'19.-25.9.'!B4</f>
         <v>PO</v>
       </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
+      <c r="C4" s="3">
+        <v>3</v>
+      </c>
+      <c r="D4" s="3">
+        <v>1</v>
+      </c>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
+      <c r="G4" s="3">
+        <v>3</v>
+      </c>
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="str">
         <f>'19.-25.9.'!A5</f>
         <v>Nikola Schönová</v>
@@ -2776,17 +2789,25 @@
         <v>3</v>
       </c>
       <c r="D5" s="3">
-        <v>1</v>
-      </c>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
+        <v>3</v>
+      </c>
+      <c r="E5" s="3">
+        <v>0</v>
+      </c>
+      <c r="F5" s="3">
+        <v>0</v>
+      </c>
       <c r="G5" s="3">
-        <v>1</v>
-      </c>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-    </row>
-    <row r="6" spans="1:9">
+        <v>4</v>
+      </c>
+      <c r="H5" s="3">
+        <v>4</v>
+      </c>
+      <c r="I5" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="str">
         <f>'19.-25.9.'!A6</f>
         <v>David Henzl</v>
@@ -2795,8 +2816,12 @@
         <f>'19.-25.9.'!B6</f>
         <v>TM</v>
       </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
+      <c r="C6" s="3">
+        <v>2</v>
+      </c>
+      <c r="D6" s="3">
+        <v>1</v>
+      </c>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
       <c r="G6" s="3">
@@ -2805,7 +2830,7 @@
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="str">
         <f>'19.-25.9.'!A7</f>
         <v>Vojtěch Kordina</v>
@@ -2814,15 +2839,29 @@
         <f>'19.-25.9.'!B7</f>
         <v>TM</v>
       </c>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-    </row>
-    <row r="8" spans="1:9">
+      <c r="C7" s="3">
+        <v>1</v>
+      </c>
+      <c r="D7" s="3">
+        <v>2</v>
+      </c>
+      <c r="E7" s="3">
+        <v>0</v>
+      </c>
+      <c r="F7" s="3">
+        <v>5</v>
+      </c>
+      <c r="G7" s="3">
+        <v>3</v>
+      </c>
+      <c r="H7" s="3">
+        <v>1</v>
+      </c>
+      <c r="I7" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="str">
         <f>'19.-25.9.'!A8</f>
         <v>Jan Matoušek</v>
@@ -2831,13 +2870,27 @@
         <f>'19.-25.9.'!B8</f>
         <v>TM</v>
       </c>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
+      <c r="C8" s="3">
+        <v>3</v>
+      </c>
+      <c r="D8" s="3">
+        <v>2</v>
+      </c>
+      <c r="E8" s="3">
+        <v>0</v>
+      </c>
+      <c r="F8" s="3">
+        <v>3</v>
+      </c>
+      <c r="G8" s="3">
+        <v>3</v>
+      </c>
+      <c r="H8" s="3">
+        <v>2</v>
+      </c>
+      <c r="I8" s="3">
+        <v>3</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -2858,13 +2911,13 @@
       <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.85546875" customWidth="1"/>
     <col min="3" max="9" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -2883,7 +2936,7 @@
       <c r="H1" s="4"/>
       <c r="I1" s="4"/>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="5"/>
       <c r="B2" s="7"/>
       <c r="C2" s="1" t="s">
@@ -2908,7 +2961,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="str">
         <f>'19.-25.9.'!A3</f>
         <v>Miroslav Vávrů</v>
@@ -2925,7 +2978,7 @@
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="str">
         <f>'19.-25.9.'!A4</f>
         <v xml:space="preserve">Tomáš Došek </v>
@@ -2942,7 +2995,7 @@
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="str">
         <f>'19.-25.9.'!A5</f>
         <v>Nikola Schönová</v>
@@ -2959,7 +3012,7 @@
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="str">
         <f>'19.-25.9.'!A6</f>
         <v>David Henzl</v>
@@ -2976,7 +3029,7 @@
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="str">
         <f>'19.-25.9.'!A7</f>
         <v>Vojtěch Kordina</v>
@@ -2993,7 +3046,7 @@
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="str">
         <f>'19.-25.9.'!A8</f>
         <v>Jan Matoušek</v>
@@ -3029,13 +3082,13 @@
       <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.85546875" customWidth="1"/>
     <col min="3" max="9" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -3054,7 +3107,7 @@
       <c r="H1" s="4"/>
       <c r="I1" s="4"/>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="5"/>
       <c r="B2" s="7"/>
       <c r="C2" s="1" t="s">
@@ -3079,7 +3132,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="str">
         <f>'19.-25.9.'!A3</f>
         <v>Miroslav Vávrů</v>
@@ -3096,7 +3149,7 @@
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="str">
         <f>'19.-25.9.'!A4</f>
         <v xml:space="preserve">Tomáš Došek </v>
@@ -3113,7 +3166,7 @@
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="str">
         <f>'19.-25.9.'!A5</f>
         <v>Nikola Schönová</v>
@@ -3130,7 +3183,7 @@
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="str">
         <f>'19.-25.9.'!A6</f>
         <v>David Henzl</v>
@@ -3147,7 +3200,7 @@
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="str">
         <f>'19.-25.9.'!A7</f>
         <v>Vojtěch Kordina</v>
@@ -3164,7 +3217,7 @@
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="str">
         <f>'19.-25.9.'!A8</f>
         <v>Jan Matoušek</v>
@@ -3200,13 +3253,13 @@
       <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.85546875" customWidth="1"/>
     <col min="3" max="9" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -3225,7 +3278,7 @@
       <c r="H1" s="4"/>
       <c r="I1" s="4"/>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="5"/>
       <c r="B2" s="7"/>
       <c r="C2" s="1" t="s">
@@ -3250,7 +3303,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="str">
         <f>'19.-25.9.'!A3</f>
         <v>Miroslav Vávrů</v>
@@ -3267,7 +3320,7 @@
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="str">
         <f>'19.-25.9.'!A4</f>
         <v xml:space="preserve">Tomáš Došek </v>
@@ -3284,7 +3337,7 @@
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="str">
         <f>'19.-25.9.'!A5</f>
         <v>Nikola Schönová</v>
@@ -3301,7 +3354,7 @@
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="str">
         <f>'19.-25.9.'!A6</f>
         <v>David Henzl</v>
@@ -3318,7 +3371,7 @@
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="str">
         <f>'19.-25.9.'!A7</f>
         <v>Vojtěch Kordina</v>
@@ -3335,7 +3388,7 @@
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="str">
         <f>'19.-25.9.'!A8</f>
         <v>Jan Matoušek</v>
@@ -3371,13 +3424,13 @@
       <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.85546875" customWidth="1"/>
     <col min="3" max="9" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -3396,7 +3449,7 @@
       <c r="H1" s="4"/>
       <c r="I1" s="4"/>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="5"/>
       <c r="B2" s="7"/>
       <c r="C2" s="1" t="s">
@@ -3421,7 +3474,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="str">
         <f>'19.-25.9.'!A3</f>
         <v>Miroslav Vávrů</v>
@@ -3438,7 +3491,7 @@
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="str">
         <f>'19.-25.9.'!A4</f>
         <v xml:space="preserve">Tomáš Došek </v>
@@ -3455,7 +3508,7 @@
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="str">
         <f>'19.-25.9.'!A5</f>
         <v>Nikola Schönová</v>
@@ -3472,7 +3525,7 @@
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="str">
         <f>'19.-25.9.'!A6</f>
         <v>David Henzl</v>
@@ -3489,7 +3542,7 @@
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="str">
         <f>'19.-25.9.'!A7</f>
         <v>Vojtěch Kordina</v>
@@ -3506,7 +3559,7 @@
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="str">
         <f>'19.-25.9.'!A8</f>
         <v>Jan Matoušek</v>
@@ -3682,13 +3735,36 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{84EB3E87-8674-4815-A2C5-3FD9C0DA0B43}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{84EB3E87-8674-4815-A2C5-3FD9C0DA0B43}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CBEB379E-111D-4A71-B78C-75057F607BED}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CBEB379E-111D-4A71-B78C-75057F607BED}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AB9D5C8D-C0CD-4FC9-A26C-36F771276680}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AB9D5C8D-C0CD-4FC9-A26C-36F771276680}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="44a14aa1-0894-4409-a040-86e619425f06"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
update navbar + týdenní správa gitu
</commit_message>
<xml_diff>
--- a/dokumentace/RSP_UNICORN_tydny_prehledy_22_JV1(1).xlsx
+++ b/dokumentace/RSP_UNICORN_tydny_prehledy_22_JV1(1).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\schonova\RSP\UNICORN\dokumentace\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BB56384-45D4-43C0-9335-B81A3D7637F9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BA70651-0B00-4617-8139-EBCE10E1C69A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" firstSheet="4" activeTab="6" xr2:uid="{BC61F073-B12C-482B-97C0-FC4A34FC5EED}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" firstSheet="4" activeTab="7" xr2:uid="{BC61F073-B12C-482B-97C0-FC4A34FC5EED}"/>
   </bookViews>
   <sheets>
     <sheet name="19.-25.9." sheetId="2" r:id="rId1"/>
@@ -1672,23 +1672,23 @@
       </c>
       <c r="E3" s="3">
         <f>'19.-25.9.'!E3+'26.9.- 2.10.'!E3+'3.10. - 9.10'!E3+'10.10 - 16.10.'!E3+'17.10. - 23.10.'!E3+'24.10. - 30.10.'!E3+'31.10. - 6.11.'!E3+'7.11. - 13.11.'!E3+'14.11. - 20.11.'!E3+'21.11. - 27.11.'!E3+'28.11. - 4.12.'!E3+'5.12. - 11.12.'!E3+'12.12. - 18.12.'!E3+'19.12. - 25.12.'!E3</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F3" s="3">
         <f>'19.-25.9.'!F3+'26.9.- 2.10.'!F3+'3.10. - 9.10'!F3+'10.10 - 16.10.'!F3+'17.10. - 23.10.'!F3+'24.10. - 30.10.'!F3+'31.10. - 6.11.'!F3+'7.11. - 13.11.'!F3+'14.11. - 20.11.'!F3+'21.11. - 27.11.'!F3+'28.11. - 4.12.'!F3+'5.12. - 11.12.'!F3+'12.12. - 18.12.'!F3+'19.12. - 25.12.'!F3</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G3" s="3">
         <f>'19.-25.9.'!G3+'26.9.- 2.10.'!G3+'3.10. - 9.10'!G3+'10.10 - 16.10.'!G3+'17.10. - 23.10.'!G3+'24.10. - 30.10.'!G3+'31.10. - 6.11.'!G3+'7.11. - 13.11.'!G3+'14.11. - 20.11.'!G3+'21.11. - 27.11.'!G3+'28.11. - 4.12.'!G3+'5.12. - 11.12.'!G3+'12.12. - 18.12.'!G3+'19.12. - 25.12.'!G3</f>
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="H3" s="3">
         <f>'19.-25.9.'!H3+'26.9.- 2.10.'!H3+'3.10. - 9.10'!H3+'10.10 - 16.10.'!H3+'17.10. - 23.10.'!H3+'24.10. - 30.10.'!H3+'31.10. - 6.11.'!H3+'7.11. - 13.11.'!H3+'14.11. - 20.11.'!H3+'21.11. - 27.11.'!H3+'28.11. - 4.12.'!H3+'5.12. - 11.12.'!H3+'12.12. - 18.12.'!H3+'19.12. - 25.12.'!H3</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I3" s="3">
         <f>'19.-25.9.'!I3+'26.9.- 2.10.'!I3+'3.10. - 9.10'!I3+'10.10 - 16.10.'!I3+'17.10. - 23.10.'!I3+'24.10. - 30.10.'!I3+'31.10. - 6.11.'!I3+'7.11. - 13.11.'!I3+'14.11. - 20.11.'!I3+'21.11. - 27.11.'!I3+'28.11. - 4.12.'!I3+'5.12. - 11.12.'!I3+'12.12. - 18.12.'!I3+'19.12. - 25.12.'!I3</f>
-        <v>17</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -1702,11 +1702,11 @@
       </c>
       <c r="C4" s="3">
         <f>'19.-25.9.'!C4+'26.9.- 2.10.'!C4+'3.10. - 9.10'!C4+'10.10 - 16.10.'!C4+'17.10. - 23.10.'!C4+'24.10. - 30.10.'!C4+'31.10. - 6.11.'!C4+'7.11. - 13.11.'!C4+'14.11. - 20.11.'!C4+'21.11. - 27.11.'!C4+'28.11. - 4.12.'!C4+'5.12. - 11.12.'!C4+'12.12. - 18.12.'!C4+'19.12. - 25.12.'!C4</f>
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="D4" s="3">
         <f>'19.-25.9.'!D4+'26.9.- 2.10.'!D4+'3.10. - 9.10'!D4+'10.10 - 16.10.'!D4+'17.10. - 23.10.'!D4+'24.10. - 30.10.'!D4+'31.10. - 6.11.'!D4+'7.11. - 13.11.'!D4+'14.11. - 20.11.'!D4+'21.11. - 27.11.'!D4+'28.11. - 4.12.'!D4+'5.12. - 11.12.'!D4+'12.12. - 18.12.'!D4+'19.12. - 25.12.'!D4</f>
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="E4" s="3">
         <f>'19.-25.9.'!E4+'26.9.- 2.10.'!E4+'3.10. - 9.10'!E4+'10.10 - 16.10.'!E4+'17.10. - 23.10.'!E4+'24.10. - 30.10.'!E4+'31.10. - 6.11.'!E4+'7.11. - 13.11.'!E4+'14.11. - 20.11.'!E4+'21.11. - 27.11.'!E4+'28.11. - 4.12.'!E4+'5.12. - 11.12.'!E4+'12.12. - 18.12.'!E4+'19.12. - 25.12.'!E4</f>
@@ -1718,15 +1718,15 @@
       </c>
       <c r="G4" s="3">
         <f>'19.-25.9.'!G4+'26.9.- 2.10.'!G4+'3.10. - 9.10'!G4+'10.10 - 16.10.'!G4+'17.10. - 23.10.'!G4+'24.10. - 30.10.'!G4+'31.10. - 6.11.'!G4+'7.11. - 13.11.'!G4+'14.11. - 20.11.'!G4+'21.11. - 27.11.'!G4+'28.11. - 4.12.'!G4+'5.12. - 11.12.'!G4+'12.12. - 18.12.'!G4+'19.12. - 25.12.'!G4</f>
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="H4" s="3">
         <f>'19.-25.9.'!H4+'26.9.- 2.10.'!H4+'3.10. - 9.10'!H4+'10.10 - 16.10.'!H4+'17.10. - 23.10.'!H4+'24.10. - 30.10.'!H4+'31.10. - 6.11.'!H4+'7.11. - 13.11.'!H4+'14.11. - 20.11.'!H4+'21.11. - 27.11.'!H4+'28.11. - 4.12.'!H4+'5.12. - 11.12.'!H4+'12.12. - 18.12.'!H4+'19.12. - 25.12.'!H4</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I4" s="3">
         <f>'19.-25.9.'!I4+'26.9.- 2.10.'!I4+'3.10. - 9.10'!I4+'10.10 - 16.10.'!I4+'17.10. - 23.10.'!I4+'24.10. - 30.10.'!I4+'31.10. - 6.11.'!I4+'7.11. - 13.11.'!I4+'14.11. - 20.11.'!I4+'21.11. - 27.11.'!I4+'28.11. - 4.12.'!I4+'5.12. - 11.12.'!I4+'12.12. - 18.12.'!I4+'19.12. - 25.12.'!I4</f>
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -1740,31 +1740,31 @@
       </c>
       <c r="C5" s="3">
         <f>'19.-25.9.'!C5+'26.9.- 2.10.'!C5+'3.10. - 9.10'!C5+'10.10 - 16.10.'!C5+'17.10. - 23.10.'!C5+'24.10. - 30.10.'!C5+'31.10. - 6.11.'!C5+'7.11. - 13.11.'!C5+'14.11. - 20.11.'!C5+'21.11. - 27.11.'!C5+'28.11. - 4.12.'!C5+'5.12. - 11.12.'!C5+'12.12. - 18.12.'!C5+'19.12. - 25.12.'!C5</f>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D5" s="3">
         <f>'19.-25.9.'!D5+'26.9.- 2.10.'!D5+'3.10. - 9.10'!D5+'10.10 - 16.10.'!D5+'17.10. - 23.10.'!D5+'24.10. - 30.10.'!D5+'31.10. - 6.11.'!D5+'7.11. - 13.11.'!D5+'14.11. - 20.11.'!D5+'21.11. - 27.11.'!D5+'28.11. - 4.12.'!D5+'5.12. - 11.12.'!D5+'12.12. - 18.12.'!D5+'19.12. - 25.12.'!D5</f>
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="E5" s="3">
         <f>'19.-25.9.'!E5+'26.9.- 2.10.'!E5+'3.10. - 9.10'!E5+'10.10 - 16.10.'!E5+'17.10. - 23.10.'!E5+'24.10. - 30.10.'!E5+'31.10. - 6.11.'!E5+'7.11. - 13.11.'!E5+'14.11. - 20.11.'!E5+'21.11. - 27.11.'!E5+'28.11. - 4.12.'!E5+'5.12. - 11.12.'!E5+'12.12. - 18.12.'!E5+'19.12. - 25.12.'!E5</f>
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="F5" s="3">
         <f>'19.-25.9.'!F5+'26.9.- 2.10.'!F5+'3.10. - 9.10'!F5+'10.10 - 16.10.'!F5+'17.10. - 23.10.'!F5+'24.10. - 30.10.'!F5+'31.10. - 6.11.'!F5+'7.11. - 13.11.'!F5+'14.11. - 20.11.'!F5+'21.11. - 27.11.'!F5+'28.11. - 4.12.'!F5+'5.12. - 11.12.'!F5+'12.12. - 18.12.'!F5+'19.12. - 25.12.'!F5</f>
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="G5" s="3">
         <f>'19.-25.9.'!G5+'26.9.- 2.10.'!G5+'3.10. - 9.10'!G5+'10.10 - 16.10.'!G5+'17.10. - 23.10.'!G5+'24.10. - 30.10.'!G5+'31.10. - 6.11.'!G5+'7.11. - 13.11.'!G5+'14.11. - 20.11.'!G5+'21.11. - 27.11.'!G5+'28.11. - 4.12.'!G5+'5.12. - 11.12.'!G5+'12.12. - 18.12.'!G5+'19.12. - 25.12.'!G5</f>
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="H5" s="3">
         <f>'19.-25.9.'!H5+'26.9.- 2.10.'!H5+'3.10. - 9.10'!H5+'10.10 - 16.10.'!H5+'17.10. - 23.10.'!H5+'24.10. - 30.10.'!H5+'31.10. - 6.11.'!H5+'7.11. - 13.11.'!H5+'14.11. - 20.11.'!H5+'21.11. - 27.11.'!H5+'28.11. - 4.12.'!H5+'5.12. - 11.12.'!H5+'12.12. - 18.12.'!H5+'19.12. - 25.12.'!H5</f>
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I5" s="3">
         <f>'19.-25.9.'!I5+'26.9.- 2.10.'!I5+'3.10. - 9.10'!I5+'10.10 - 16.10.'!I5+'17.10. - 23.10.'!I5+'24.10. - 30.10.'!I5+'31.10. - 6.11.'!I5+'7.11. - 13.11.'!I5+'14.11. - 20.11.'!I5+'21.11. - 27.11.'!I5+'28.11. - 4.12.'!I5+'5.12. - 11.12.'!I5+'12.12. - 18.12.'!I5+'19.12. - 25.12.'!I5</f>
-        <v>25</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -1778,11 +1778,11 @@
       </c>
       <c r="C6" s="3">
         <f>'19.-25.9.'!C6+'26.9.- 2.10.'!C6+'3.10. - 9.10'!C6+'10.10 - 16.10.'!C6+'17.10. - 23.10.'!C6+'24.10. - 30.10.'!C6+'31.10. - 6.11.'!C6+'7.11. - 13.11.'!C6+'14.11. - 20.11.'!C6+'21.11. - 27.11.'!C6+'28.11. - 4.12.'!C6+'5.12. - 11.12.'!C6+'12.12. - 18.12.'!C6+'19.12. - 25.12.'!C6</f>
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D6" s="3">
         <f>'19.-25.9.'!D6+'26.9.- 2.10.'!D6+'3.10. - 9.10'!D6+'10.10 - 16.10.'!D6+'17.10. - 23.10.'!D6+'24.10. - 30.10.'!D6+'31.10. - 6.11.'!D6+'7.11. - 13.11.'!D6+'14.11. - 20.11.'!D6+'21.11. - 27.11.'!D6+'28.11. - 4.12.'!D6+'5.12. - 11.12.'!D6+'12.12. - 18.12.'!D6+'19.12. - 25.12.'!D6</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E6" s="3">
         <f>'19.-25.9.'!E6+'26.9.- 2.10.'!E6+'3.10. - 9.10'!E6+'10.10 - 16.10.'!E6+'17.10. - 23.10.'!E6+'24.10. - 30.10.'!E6+'31.10. - 6.11.'!E6+'7.11. - 13.11.'!E6+'14.11. - 20.11.'!E6+'21.11. - 27.11.'!E6+'28.11. - 4.12.'!E6+'5.12. - 11.12.'!E6+'12.12. - 18.12.'!E6+'19.12. - 25.12.'!E6</f>
@@ -1794,7 +1794,7 @@
       </c>
       <c r="G6" s="3">
         <f>'19.-25.9.'!G6+'26.9.- 2.10.'!G6+'3.10. - 9.10'!G6+'10.10 - 16.10.'!G6+'17.10. - 23.10.'!G6+'24.10. - 30.10.'!G6+'31.10. - 6.11.'!G6+'7.11. - 13.11.'!G6+'14.11. - 20.11.'!G6+'21.11. - 27.11.'!G6+'28.11. - 4.12.'!G6+'5.12. - 11.12.'!G6+'12.12. - 18.12.'!G6+'19.12. - 25.12.'!G6</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H6" s="3">
         <f>'19.-25.9.'!H6+'26.9.- 2.10.'!H6+'3.10. - 9.10'!H6+'10.10 - 16.10.'!H6+'17.10. - 23.10.'!H6+'24.10. - 30.10.'!H6+'31.10. - 6.11.'!H6+'7.11. - 13.11.'!H6+'14.11. - 20.11.'!H6+'21.11. - 27.11.'!H6+'28.11. - 4.12.'!H6+'5.12. - 11.12.'!H6+'12.12. - 18.12.'!H6+'19.12. - 25.12.'!H6</f>
@@ -1816,31 +1816,31 @@
       </c>
       <c r="C7" s="3">
         <f>'19.-25.9.'!C7+'26.9.- 2.10.'!C7+'3.10. - 9.10'!C7+'10.10 - 16.10.'!C7+'17.10. - 23.10.'!C7+'24.10. - 30.10.'!C7+'31.10. - 6.11.'!C7+'7.11. - 13.11.'!C7+'14.11. - 20.11.'!C7+'21.11. - 27.11.'!C7+'28.11. - 4.12.'!C7+'5.12. - 11.12.'!C7+'12.12. - 18.12.'!C7+'19.12. - 25.12.'!C7</f>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D7" s="3">
         <f>'19.-25.9.'!D7+'26.9.- 2.10.'!D7+'3.10. - 9.10'!D7+'10.10 - 16.10.'!D7+'17.10. - 23.10.'!D7+'24.10. - 30.10.'!D7+'31.10. - 6.11.'!D7+'7.11. - 13.11.'!D7+'14.11. - 20.11.'!D7+'21.11. - 27.11.'!D7+'28.11. - 4.12.'!D7+'5.12. - 11.12.'!D7+'12.12. - 18.12.'!D7+'19.12. - 25.12.'!D7</f>
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E7" s="3">
         <f>'19.-25.9.'!E7+'26.9.- 2.10.'!E7+'3.10. - 9.10'!E7+'10.10 - 16.10.'!E7+'17.10. - 23.10.'!E7+'24.10. - 30.10.'!E7+'31.10. - 6.11.'!E7+'7.11. - 13.11.'!E7+'14.11. - 20.11.'!E7+'21.11. - 27.11.'!E7+'28.11. - 4.12.'!E7+'5.12. - 11.12.'!E7+'12.12. - 18.12.'!E7+'19.12. - 25.12.'!E7</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F7" s="3">
         <f>'19.-25.9.'!F7+'26.9.- 2.10.'!F7+'3.10. - 9.10'!F7+'10.10 - 16.10.'!F7+'17.10. - 23.10.'!F7+'24.10. - 30.10.'!F7+'31.10. - 6.11.'!F7+'7.11. - 13.11.'!F7+'14.11. - 20.11.'!F7+'21.11. - 27.11.'!F7+'28.11. - 4.12.'!F7+'5.12. - 11.12.'!F7+'12.12. - 18.12.'!F7+'19.12. - 25.12.'!F7</f>
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="G7" s="3">
         <f>'19.-25.9.'!G7+'26.9.- 2.10.'!G7+'3.10. - 9.10'!G7+'10.10 - 16.10.'!G7+'17.10. - 23.10.'!G7+'24.10. - 30.10.'!G7+'31.10. - 6.11.'!G7+'7.11. - 13.11.'!G7+'14.11. - 20.11.'!G7+'21.11. - 27.11.'!G7+'28.11. - 4.12.'!G7+'5.12. - 11.12.'!G7+'12.12. - 18.12.'!G7+'19.12. - 25.12.'!G7</f>
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="H7" s="3">
         <f>'19.-25.9.'!H7+'26.9.- 2.10.'!H7+'3.10. - 9.10'!H7+'10.10 - 16.10.'!H7+'17.10. - 23.10.'!H7+'24.10. - 30.10.'!H7+'31.10. - 6.11.'!H7+'7.11. - 13.11.'!H7+'14.11. - 20.11.'!H7+'21.11. - 27.11.'!H7+'28.11. - 4.12.'!H7+'5.12. - 11.12.'!H7+'12.12. - 18.12.'!H7+'19.12. - 25.12.'!H7</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I7" s="3">
         <f>'19.-25.9.'!I7+'26.9.- 2.10.'!I7+'3.10. - 9.10'!I7+'10.10 - 16.10.'!I7+'17.10. - 23.10.'!I7+'24.10. - 30.10.'!I7+'31.10. - 6.11.'!I7+'7.11. - 13.11.'!I7+'14.11. - 20.11.'!I7+'21.11. - 27.11.'!I7+'28.11. - 4.12.'!I7+'5.12. - 11.12.'!I7+'12.12. - 18.12.'!I7+'19.12. - 25.12.'!I7</f>
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -1854,31 +1854,31 @@
       </c>
       <c r="C8" s="3">
         <f>'19.-25.9.'!C8+'26.9.- 2.10.'!C8+'3.10. - 9.10'!C8+'10.10 - 16.10.'!C8+'17.10. - 23.10.'!C8+'24.10. - 30.10.'!C8+'31.10. - 6.11.'!C8+'7.11. - 13.11.'!C8+'14.11. - 20.11.'!C8+'21.11. - 27.11.'!C8+'28.11. - 4.12.'!C8+'5.12. - 11.12.'!C8+'12.12. - 18.12.'!C8+'19.12. - 25.12.'!C8</f>
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D8" s="3">
         <f>'19.-25.9.'!D8+'26.9.- 2.10.'!D8+'3.10. - 9.10'!D8+'10.10 - 16.10.'!D8+'17.10. - 23.10.'!D8+'24.10. - 30.10.'!D8+'31.10. - 6.11.'!D8+'7.11. - 13.11.'!D8+'14.11. - 20.11.'!D8+'21.11. - 27.11.'!D8+'28.11. - 4.12.'!D8+'5.12. - 11.12.'!D8+'12.12. - 18.12.'!D8+'19.12. - 25.12.'!D8</f>
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="E8" s="3">
         <f>'19.-25.9.'!E8+'26.9.- 2.10.'!E8+'3.10. - 9.10'!E8+'10.10 - 16.10.'!E8+'17.10. - 23.10.'!E8+'24.10. - 30.10.'!E8+'31.10. - 6.11.'!E8+'7.11. - 13.11.'!E8+'14.11. - 20.11.'!E8+'21.11. - 27.11.'!E8+'28.11. - 4.12.'!E8+'5.12. - 11.12.'!E8+'12.12. - 18.12.'!E8+'19.12. - 25.12.'!E8</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F8" s="3">
         <f>'19.-25.9.'!F8+'26.9.- 2.10.'!F8+'3.10. - 9.10'!F8+'10.10 - 16.10.'!F8+'17.10. - 23.10.'!F8+'24.10. - 30.10.'!F8+'31.10. - 6.11.'!F8+'7.11. - 13.11.'!F8+'14.11. - 20.11.'!F8+'21.11. - 27.11.'!F8+'28.11. - 4.12.'!F8+'5.12. - 11.12.'!F8+'12.12. - 18.12.'!F8+'19.12. - 25.12.'!F8</f>
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="G8" s="3">
         <f>'19.-25.9.'!G8+'26.9.- 2.10.'!G8+'3.10. - 9.10'!G8+'10.10 - 16.10.'!G8+'17.10. - 23.10.'!G8+'24.10. - 30.10.'!G8+'31.10. - 6.11.'!G8+'7.11. - 13.11.'!G8+'14.11. - 20.11.'!G8+'21.11. - 27.11.'!G8+'28.11. - 4.12.'!G8+'5.12. - 11.12.'!G8+'12.12. - 18.12.'!G8+'19.12. - 25.12.'!G8</f>
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="H8" s="3">
         <f>'19.-25.9.'!H8+'26.9.- 2.10.'!H8+'3.10. - 9.10'!H8+'10.10 - 16.10.'!H8+'17.10. - 23.10.'!H8+'24.10. - 30.10.'!H8+'31.10. - 6.11.'!H8+'7.11. - 13.11.'!H8+'14.11. - 20.11.'!H8+'21.11. - 27.11.'!H8+'28.11. - 4.12.'!H8+'5.12. - 11.12.'!H8+'12.12. - 18.12.'!H8+'19.12. - 25.12.'!H8</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I8" s="3">
         <f>'19.-25.9.'!I8+'26.9.- 2.10.'!I8+'3.10. - 9.10'!I8+'10.10 - 16.10.'!I8+'17.10. - 23.10.'!I8+'24.10. - 30.10.'!I8+'31.10. - 6.11.'!I8+'7.11. - 13.11.'!I8+'14.11. - 20.11.'!I8+'21.11. - 27.11.'!I8+'28.11. - 4.12.'!I8+'5.12. - 11.12.'!I8+'12.12. - 18.12.'!I8+'19.12. - 25.12.'!I8</f>
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -1888,31 +1888,31 @@
       <c r="B9" s="9"/>
       <c r="C9" s="1">
         <f>SUM(C3:C8)</f>
-        <v>95</v>
+        <v>107</v>
       </c>
       <c r="D9" s="1">
         <f t="shared" ref="D9:I9" si="0">SUM(D3:D8)</f>
-        <v>71</v>
+        <v>89</v>
       </c>
       <c r="E9" s="1">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="F9" s="1">
         <f t="shared" si="0"/>
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="G9" s="1">
         <f t="shared" si="0"/>
-        <v>65</v>
+        <v>89</v>
       </c>
       <c r="H9" s="1">
         <f t="shared" si="0"/>
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="I9" s="1">
         <f t="shared" si="0"/>
-        <v>75</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -2921,8 +2921,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FF5DD16-DA71-473A-A921-ACA553B76744}">
   <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3015,11 +3015,17 @@
         <f>'19.-25.9.'!B4</f>
         <v>PO</v>
       </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
+      <c r="C4" s="3">
+        <v>3</v>
+      </c>
+      <c r="D4" s="3">
+        <v>1</v>
+      </c>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
+      <c r="G4" s="3">
+        <v>3</v>
+      </c>
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
     </row>
@@ -3063,11 +3069,17 @@
         <f>'19.-25.9.'!B6</f>
         <v>TM</v>
       </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
+      <c r="C6" s="3">
+        <v>2</v>
+      </c>
+      <c r="D6" s="3">
+        <v>1</v>
+      </c>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
+      <c r="G6" s="3">
+        <v>1</v>
+      </c>
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
     </row>
@@ -3148,8 +3160,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{989920D2-ECE5-42E0-BC55-8E2FB1FA70A4}">
   <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3217,11 +3229,21 @@
       <c r="D3" s="3">
         <v>1</v>
       </c>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
+      <c r="E3" s="3">
+        <v>0</v>
+      </c>
+      <c r="F3" s="3">
+        <v>2</v>
+      </c>
+      <c r="G3" s="3">
+        <v>3</v>
+      </c>
+      <c r="H3" s="3">
+        <v>1</v>
+      </c>
+      <c r="I3" s="3">
+        <v>7</v>
+      </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="str">
@@ -3232,13 +3254,27 @@
         <f>'19.-25.9.'!B4</f>
         <v>PO</v>
       </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
+      <c r="C4" s="3">
+        <v>2</v>
+      </c>
+      <c r="D4" s="3">
+        <v>5</v>
+      </c>
+      <c r="E4" s="3">
+        <v>0</v>
+      </c>
+      <c r="F4" s="3">
+        <v>0</v>
+      </c>
+      <c r="G4" s="3">
+        <v>4</v>
+      </c>
+      <c r="H4" s="3">
+        <v>1</v>
+      </c>
+      <c r="I4" s="3">
+        <v>5</v>
+      </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="str">
@@ -3255,10 +3291,14 @@
       <c r="D5" s="3">
         <v>2</v>
       </c>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
+      <c r="E5" s="3">
+        <v>5</v>
+      </c>
+      <c r="F5" s="3">
+        <v>5</v>
+      </c>
       <c r="G5" s="3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H5" s="3">
         <v>2</v>
@@ -3293,13 +3333,27 @@
         <f>'19.-25.9.'!B7</f>
         <v>TM</v>
       </c>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
+      <c r="C7" s="3">
+        <v>2</v>
+      </c>
+      <c r="D7" s="3">
+        <v>4</v>
+      </c>
+      <c r="E7" s="3">
+        <v>1</v>
+      </c>
+      <c r="F7" s="3">
+        <v>4</v>
+      </c>
+      <c r="G7" s="3">
+        <v>3</v>
+      </c>
+      <c r="H7" s="3">
+        <v>1</v>
+      </c>
+      <c r="I7" s="3">
+        <v>3</v>
+      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="str">
@@ -3310,13 +3364,27 @@
         <f>'19.-25.9.'!B8</f>
         <v>TM</v>
       </c>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
+      <c r="C8" s="3">
+        <v>2</v>
+      </c>
+      <c r="D8" s="3">
+        <v>3</v>
+      </c>
+      <c r="E8" s="3">
+        <v>2</v>
+      </c>
+      <c r="F8" s="3">
+        <v>3</v>
+      </c>
+      <c r="G8" s="3">
+        <v>3</v>
+      </c>
+      <c r="H8" s="3">
+        <v>1</v>
+      </c>
+      <c r="I8" s="3">
+        <v>3</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -3333,8 +3401,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{182703F4-F8E0-4A1D-ABD5-4B71E9E48AE6}">
   <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3398,11 +3466,17 @@
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
+      <c r="E3" s="3">
+        <v>1</v>
+      </c>
       <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
+      <c r="G3" s="3">
+        <v>1</v>
+      </c>
       <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
+      <c r="I3" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="str">
@@ -3430,13 +3504,27 @@
         <f>'19.-25.9.'!B5</f>
         <v>TM</v>
       </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
+      <c r="C5" s="3">
+        <v>1</v>
+      </c>
+      <c r="D5" s="3">
+        <v>4</v>
+      </c>
+      <c r="E5" s="3">
+        <v>5</v>
+      </c>
+      <c r="F5" s="3">
+        <v>1</v>
+      </c>
+      <c r="G5" s="3">
+        <v>5</v>
+      </c>
+      <c r="H5" s="3">
+        <v>3</v>
+      </c>
+      <c r="I5" s="3">
+        <v>7</v>
+      </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="str">
@@ -3672,6 +3760,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100ACB71971B47CD0439EBDA2CFA6075C38" ma:contentTypeVersion="2" ma:contentTypeDescription="Vytvoří nový dokument" ma:contentTypeScope="" ma:versionID="be70910a1115bd952827b69f266b3190">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="44a14aa1-0894-4409-a040-86e619425f06" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0c08dc4d6a52cc18bfb05fd3cb1142cf" ns2:_="">
     <xsd:import namespace="44a14aa1-0894-4409-a040-86e619425f06"/>
@@ -3803,22 +3906,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{84EB3E87-8674-4815-A2C5-3FD9C0DA0B43}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CBEB379E-111D-4A71-B78C-75057F607BED}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AB9D5C8D-C0CD-4FC9-A26C-36F771276680}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3834,21 +3939,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CBEB379E-111D-4A71-B78C-75057F607BED}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{84EB3E87-8674-4815-A2C5-3FD9C0DA0B43}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>